<commit_message>
Updated for Sprint #2
</commit_message>
<xml_diff>
--- a/docs/logbooks/TButzin - Efforts Logbook.xlsx
+++ b/docs/logbooks/TButzin - Efforts Logbook.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Troy\Documents\HOMEWORK\CAPSTONE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Troy\Documents\HOMEWORK\CAPSTONE\Sprint #2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4356F26-A78B-41B8-8894-2AD3465D8289}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D73DB7-B81B-4FBE-811E-E92DC1430FFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1575" yWindow="3195" windowWidth="28800" windowHeight="17595" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t>Brief Description of Acomplishments</t>
   </si>
@@ -173,6 +173,21 @@
   </si>
   <si>
     <t>All for both files</t>
+  </si>
+  <si>
+    <t>A, B, D, E, F, I, K, N</t>
+  </si>
+  <si>
+    <t>Multiple Team meetings, along with Conference call with TARDEC, established basic website template, User stories for frontend</t>
+  </si>
+  <si>
+    <t>userstories_master, SkyPIsite, ui_user_stories</t>
+  </si>
+  <si>
+    <t>ui_user_stories.txt, userstories_master.txt, SkyPIsite directory</t>
+  </si>
+  <si>
+    <t>Both User Stories files frontend sections, SkyPIsite folder was our first template but has recently been updated with a newer template (view commits in GitHub for more details)</t>
   </si>
 </sst>
 </file>
@@ -329,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -362,34 +377,37 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -687,7 +705,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -703,40 +721,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="24"/>
       <c r="C3" s="6" t="s">
         <v>9</v>
       </c>
@@ -757,10 +775,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="16"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="7">
         <v>3.5</v>
       </c>
@@ -780,23 +798,35 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="8">
+        <v>16</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="4"/>
@@ -805,10 +835,10 @@
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="16"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="4"/>
@@ -817,10 +847,10 @@
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="16"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="4"/>
@@ -829,10 +859,10 @@
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="16"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="4"/>
@@ -841,10 +871,10 @@
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="16"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="4"/>
@@ -853,10 +883,10 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="16"/>
+      <c r="B11" s="19"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="4"/>
@@ -865,10 +895,10 @@
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="16"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="4"/>
@@ -877,10 +907,10 @@
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="16"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="4"/>
@@ -889,10 +919,10 @@
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="16"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="4"/>
@@ -901,10 +931,10 @@
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="16"/>
+      <c r="B15" s="19"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="4"/>
@@ -914,11 +944,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A2:B2"/>
@@ -932,6 +957,11 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -955,68 +985,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="26" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
     </row>
     <row r="2" spans="1:16" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="19"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="22"/>
     </row>
     <row r="3" spans="1:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="25" t="s">
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
     </row>
     <row r="4" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">

</xml_diff>

<commit_message>
Sprint #3 Updated Logbook
</commit_message>
<xml_diff>
--- a/docs/logbooks/TButzin - Efforts Logbook.xlsx
+++ b/docs/logbooks/TButzin - Efforts Logbook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Troy\Documents\HOMEWORK\CAPSTONE\Sprint #2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Troy\Documents\HOMEWORK\CAPSTONE\Sprint #3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D73DB7-B81B-4FBE-811E-E92DC1430FFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F112AD3F-6C0D-4B1A-B139-DC54ADAF5A84}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1575" yWindow="3195" windowWidth="28800" windowHeight="17595" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
   <si>
     <t>Brief Description of Acomplishments</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Team Member</t>
   </si>
   <si>
-    <t>Joe, Smith</t>
-  </si>
-  <si>
     <t>Towards objectives</t>
   </si>
   <si>
@@ -109,9 +106,6 @@
     <t>Your Name</t>
   </si>
   <si>
-    <t>John Doe</t>
-  </si>
-  <si>
     <t>Sprint#</t>
   </si>
   <si>
@@ -151,9 +145,6 @@
     <t>Sprint # 12</t>
   </si>
   <si>
-    <t>Example Project</t>
-  </si>
-  <si>
     <t>SkyPI</t>
   </si>
   <si>
@@ -188,6 +179,24 @@
   </si>
   <si>
     <t>Both User Stories files frontend sections, SkyPIsite folder was our first template but has recently been updated with a newer template (view commits in GitHub for more details)</t>
+  </si>
+  <si>
+    <t>A, C, D, G, H, J, L, M</t>
+  </si>
+  <si>
+    <t>Multiple Team meetings, In-person meeting with TARDEC, redid site Dashboard/Landing, User stories for frontend</t>
+  </si>
+  <si>
+    <t>Added/Worked on user stories, Added basic aesthetics to landing page, put basic manual tables on dashboard</t>
+  </si>
+  <si>
+    <t>SkyPi</t>
+  </si>
+  <si>
+    <t>Dashboard, Landing, userstories_master, Plaintable, Stripetable</t>
+  </si>
+  <si>
+    <t>Dashboard.js, Landing.js, userstories_master.txt, Stripetable.js, Plaintable.js</t>
   </si>
 </sst>
 </file>
@@ -722,11 +731,11 @@
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D1" s="18"/>
       <c r="E1" s="18"/>
@@ -740,7 +749,7 @@
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="22"/>
@@ -752,14 +761,14 @@
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" s="24"/>
       <c r="C3" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
@@ -776,67 +785,79 @@
     </row>
     <row r="4" spans="1:8" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="7">
         <v>3.5</v>
       </c>
       <c r="D4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="8">
         <v>16</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="H5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="14" t="s">
+    </row>
+    <row r="6" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="8">
+        <v>16</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="E6" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="F6" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="14" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="8"/>
@@ -848,7 +869,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="8"/>
@@ -860,7 +881,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="8"/>
@@ -872,7 +893,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="8"/>
@@ -884,7 +905,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="8"/>
@@ -896,7 +917,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B12" s="19"/>
       <c r="C12" s="8"/>
@@ -908,7 +929,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" s="19"/>
       <c r="C13" s="8"/>
@@ -920,7 +941,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" s="19"/>
       <c r="C14" s="8"/>
@@ -932,7 +953,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="8"/>
@@ -972,7 +993,7 @@
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -986,11 +1007,11 @@
   <sheetData>
     <row r="1" spans="1:16" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="27" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D1" s="27"/>
       <c r="E1" s="27"/>
@@ -1012,7 +1033,7 @@
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="20" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
@@ -1032,7 +1053,7 @@
       <c r="A3" s="25"/>
       <c r="B3" s="25"/>
       <c r="C3" s="26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="26"/>
       <c r="E3" s="26"/>
@@ -1050,52 +1071,52 @@
     </row>
     <row r="4" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="F4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="K4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="L4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="M4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="N4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="O4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="P4" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="P4" s="9" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="5" customFormat="1" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1103,60 +1124,38 @@
         <v>0</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="11">
-        <v>2</v>
-      </c>
-      <c r="D5" s="11">
-        <v>3</v>
-      </c>
-      <c r="E5" s="13">
-        <v>1</v>
-      </c>
-      <c r="F5" s="11">
-        <v>1</v>
-      </c>
-      <c r="G5" s="11">
-        <v>5</v>
-      </c>
-      <c r="H5" s="11">
-        <v>2</v>
-      </c>
-      <c r="I5" s="11">
-        <v>3</v>
-      </c>
-      <c r="J5" s="11">
-        <v>2</v>
-      </c>
-      <c r="K5" s="11">
-        <v>6</v>
-      </c>
-      <c r="L5" s="11">
-        <v>3</v>
-      </c>
-      <c r="M5" s="11">
-        <v>1</v>
-      </c>
-      <c r="N5" s="11">
-        <v>1</v>
-      </c>
-      <c r="O5" s="11">
-        <v>5</v>
-      </c>
-      <c r="P5" s="11">
-        <v>1</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
     </row>
     <row r="6" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>1</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
+      <c r="D6" s="8">
+        <v>1</v>
+      </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="F6" s="8">
+        <v>1</v>
+      </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -1166,46 +1165,84 @@
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
+      <c r="P6" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>2</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
+      <c r="B7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1</v>
+      </c>
+      <c r="D7" s="8">
+        <v>2</v>
+      </c>
       <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="F7" s="8">
+        <v>2</v>
+      </c>
+      <c r="G7" s="8">
+        <v>1</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1</v>
+      </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
+      <c r="K7" s="8">
+        <v>1</v>
+      </c>
       <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
+      <c r="M7" s="8">
+        <v>1</v>
+      </c>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
+      <c r="P7" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>3</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
+      <c r="B8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="8">
+        <v>2</v>
+      </c>
       <c r="D8" s="8"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="8">
+        <v>3</v>
+      </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
+      <c r="I8" s="8">
+        <v>1</v>
+      </c>
+      <c r="J8" s="8">
+        <v>1</v>
+      </c>
       <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
+      <c r="L8" s="8">
+        <v>1</v>
+      </c>
       <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
+      <c r="N8" s="8">
+        <v>1</v>
+      </c>
+      <c r="O8" s="8">
+        <v>1</v>
+      </c>
       <c r="P8" s="4"/>
     </row>
     <row r="9" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>